<commit_message>
Add readme file to small water distribution model
</commit_message>
<xml_diff>
--- a/SmallWaterDistributionModel/data/water.xlsx
+++ b/SmallWaterDistributionModel/data/water.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Adam_Project\GAMS_Code\Water\Hydra\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Apps\demos\SmallWaterDistributionModel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -134,9 +134,6 @@
     <t>Water Distribution</t>
   </si>
   <si>
-    <t>water_distribution</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>minimum diameter of pipe (m)</t>
+  </si>
+  <si>
+    <t>SmallWaterDistributionModel</t>
   </si>
 </sst>
 </file>
@@ -724,7 +724,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,13 +771,13 @@
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>21</v>
@@ -838,22 +838,22 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>37</v>
       </c>
       <c r="L3">
         <v>0.15</v>
@@ -865,7 +865,7 @@
         <v>5.33</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -904,13 +904,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -918,15 +918,15 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -937,33 +937,33 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -994,13 +994,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,15 +1008,15 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1027,33 +1027,33 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1096,31 +1096,31 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1128,33 +1128,33 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1183,105 +1183,105 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P4" t="s">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1332,25 +1332,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1358,27 +1358,27 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1401,81 +1401,81 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1586,16 +1586,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>1.212</v>
@@ -1604,21 +1604,21 @@
         <v>3.02</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>59</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
       </c>
       <c r="F4" s="1">
         <v>3.25</v>
@@ -1633,21 +1633,21 @@
         <v>1.02</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
         <v>0.45600000000000002</v>
@@ -1656,21 +1656,21 @@
         <v>6.3</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1">
         <v>6.5</v>
@@ -1685,7 +1685,7 @@
         <v>1.02</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1693,13 +1693,13 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
         <v>0.65200000000000002</v>
@@ -1708,21 +1708,21 @@
         <v>1.5</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1">
         <v>0.252</v>
@@ -1731,21 +1731,21 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1">
         <v>0.245</v>
@@ -1754,21 +1754,21 @@
         <v>4.2</v>
       </c>
       <c r="L9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1">
         <v>0.45200000000000001</v>
@@ -1777,7 +1777,7 @@
         <v>5.16</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1839,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
@@ -1876,21 +1876,21 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
@@ -1898,54 +1898,54 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>26</v>
@@ -1953,79 +1953,79 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2116,7 +2116,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2165,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2193,7 +2193,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2235,7 +2235,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,7 +2291,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2305,7 +2305,7 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2333,7 +2333,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2431,12 +2431,12 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -2445,12 +2445,12 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2459,7 +2459,7 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2483,10 +2483,10 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2517,144 +2517,144 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2662,115 +2662,115 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2813,13 +2813,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,15 +2827,15 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -2846,33 +2846,33 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>